<commit_message>
emplemented filling basic info with xlsx-populate
</commit_message>
<xml_diff>
--- a/data/dsr-template.xlsx
+++ b/data/dsr-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ferdinand/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ferdinand/Desktop/2020-projects/mcb-gas-station-manager-back/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ED183A-00F4-424F-A374-4C657AAFAA59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDCDA62-586E-9C4A-A951-04466D0F10BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,16 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">template!$A$1:$L$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -167,7 +177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -177,6 +187,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -189,6 +200,20 @@
     <font>
       <b/>
       <sz val="8"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -288,13 +313,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -306,8 +327,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -316,15 +345,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,10 +578,10 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:C31"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" zeroHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
@@ -565,980 +595,981 @@
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="18.5" customWidth="1"/>
     <col min="12" max="12" width="14.5" customWidth="1"/>
+    <col min="13" max="15" width="0" hidden="1" customWidth="1"/>
     <col min="16" max="16384" width="14.5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="10"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="10"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="6" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="4" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="5">
         <f>SUM(L7:L10)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="7">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="5">
         <f t="shared" ref="G8:G10" si="0">C8-D8</f>
         <v>0</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <f t="shared" ref="H8:H10" si="1">G8-E8</f>
         <v>0</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5">
         <f>H8*C2</f>
         <v>0</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="5">
         <f t="shared" ref="J8:J10" si="2">F8*H8</f>
         <v>0</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="5">
         <f>SUM(I8:I10,I14:I16)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="7">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="5">
         <f>H9*E2</f>
         <v>0</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="7">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="5">
         <f>H10*D2</f>
         <v>0</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="K13" s="2"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="7">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="5">
         <f t="shared" ref="G14:G16" si="3">C14-D14</f>
         <v>0</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="5">
         <f t="shared" ref="H14:H16" si="4">G14-E14</f>
         <v>0</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="5">
         <f>H14*D2</f>
         <v>0</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <f t="shared" ref="J14:J16" si="5">F14*H14</f>
         <v>0</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="K14" s="2"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="7">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="5">
         <f>H15*E2</f>
         <v>0</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="K15" s="2"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="7">
+      <c r="B16" s="5"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="5">
         <f>H16*C2</f>
         <v>0</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="K16" s="2"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="4" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="5">
         <f>SUM(L19:L22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="7">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="5">
         <f t="shared" ref="G20:G22" si="6">C20-D20</f>
         <v>0</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="5">
         <f t="shared" ref="H20:H22" si="7">G20-E20</f>
         <v>0</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="5">
         <f>H20*C3</f>
         <v>0</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="5">
         <f t="shared" ref="J20:J22" si="8">F20*H20</f>
         <v>0</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="5">
         <f>SUM(I20:I22,I26:I28)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="7">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="5">
         <f>H21*E3</f>
         <v>0</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="7">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="5">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="5">
         <f>H22*D3</f>
         <v>0</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="5">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L22" s="7"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="7"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="6" t="s">
+      <c r="I25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J25" s="6" t="s">
+      <c r="J25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K25" s="4"/>
-      <c r="L25" s="7"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+      <c r="K25" s="2"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="7">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="5">
         <f t="shared" ref="G26:G28" si="9">C26-D26</f>
         <v>0</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="5">
         <f t="shared" ref="H26:H28" si="10">G26-E26</f>
         <v>0</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="5">
         <f>H26*D3</f>
         <v>0</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="5">
         <f t="shared" ref="J26:J28" si="11">F26*H26</f>
         <v>0</v>
       </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="7"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="K26" s="2"/>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="7">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="5">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="5">
         <f>H27*E3</f>
         <v>0</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="5">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K27" s="4"/>
-      <c r="L27" s="7"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="K27" s="2"/>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="7">
+      <c r="B28" s="5"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="5">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="5">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="5">
         <f>H28*C3</f>
         <v>0</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="5">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K28" s="4"/>
-      <c r="L28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="K28" s="2"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="5" t="s">
+      <c r="E30" s="16"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="2">
         <f>SUM(H28,H20,H16,H8)</f>
         <v>0</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="2">
         <f>SUM(J28,J20,J16,J8)</f>
         <v>0</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="5">
         <f>SUM(H26,H22,H14,H10)</f>
         <v>0</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="5">
         <f>SUM(J10,J14,J22,J26)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="7">
+      <c r="B34" s="5">
         <f>SUM(H27,H21,H15,H9)</f>
         <v>0</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="5">
         <f>SUM(J27,J21,J15,J9)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1"/>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="4"/>
+      <c r="B36" s="2"/>
       <c r="D36" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="12"/>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H36" s="7"/>
-      <c r="J36" s="4" t="s">
+      <c r="H36" s="5"/>
+      <c r="J36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K36" s="7"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A37" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="D37" s="4" t="s">
+      <c r="B37" s="2"/>
+      <c r="D37" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="J37" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="K37" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A38" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+      <c r="B38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="5">
         <f>B36*B37+B38</f>
         <v>0</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="5">
         <f>SUM(E53,H53)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-    </row>
-    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-    </row>
-    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" ht="16">
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" ht="16">
+      <c r="A42" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-    </row>
-    <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="B42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" ht="16">
+      <c r="A43" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-    </row>
-    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="4">
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" ht="16">
+      <c r="A44" s="2">
         <v>1000</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-    </row>
-    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="4">
+      <c r="B44" s="6"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="1:11" ht="16">
+      <c r="A45" s="2">
         <v>500</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-    </row>
-    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="4">
+      <c r="B45" s="6"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+    </row>
+    <row r="46" spans="1:11" ht="16">
+      <c r="A46" s="2">
         <v>200</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-    </row>
-    <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
+      <c r="B46" s="6"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="1:11" ht="16">
+      <c r="A47" s="2">
         <v>100</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="4"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="4"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="4"/>
-    </row>
-    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
+      <c r="B47" s="6"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="2"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="2"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" ht="16">
+      <c r="A48" s="2">
         <v>50</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
+      <c r="B48" s="6"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:11" ht="16">
+      <c r="A49" s="2">
         <v>20</v>
       </c>
-      <c r="B49" s="8"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-    </row>
-    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
+      <c r="B49" s="6"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="1:11" ht="16">
+      <c r="A50" s="2">
         <v>10</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-    </row>
-    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
+      <c r="B50" s="6"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:11" ht="16">
+      <c r="A51" s="2">
         <v>5</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
+      <c r="B51" s="6"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:11" ht="16">
+      <c r="A52" s="2">
         <v>1</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-    </row>
-    <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
+      <c r="B52" s="6"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" ht="16">
+      <c r="A53" s="2">
         <v>0.25</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="7">
+      <c r="B53" s="6"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="5">
         <f>SUM(E38:E52)</f>
         <v>0</v>
       </c>
-      <c r="G53" s="4"/>
-      <c r="H53" s="7">
+      <c r="G53" s="2"/>
+      <c r="H53" s="5">
         <f>SUM(H38:H52)</f>
         <v>0</v>
       </c>
-      <c r="J53" s="4"/>
-      <c r="K53" s="7">
+      <c r="J53" s="2"/>
+      <c r="K53" s="5">
         <f>SUM(K38:K52)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
finished: sales summary for each day
</commit_message>
<xml_diff>
--- a/data/dsr-template.xlsx
+++ b/data/dsr-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ferdinand/Desktop/2020-projects/mcb-gas-station-manager-back/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD50EA5-3A33-C647-BBAC-4AD9921C50D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE31FD35-8813-9347-A179-B157F958622D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dsr-template" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="56">
   <si>
     <t>DATE</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>OUTSIDE EXPENSES</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -422,33 +419,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -474,6 +448,29 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1377,24 +1374,24 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1"/>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="16"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="14"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="31"/>
       <c r="D31" s="3" t="s">
         <v>28</v>
       </c>
@@ -1453,10 +1450,10 @@
         <v>30</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="12"/>
+      <c r="E36" s="29"/>
       <c r="G36" s="2" t="s">
         <v>36</v>
       </c>
@@ -1713,1012 +1710,1010 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="9" width="14.5" style="19"/>
-    <col min="10" max="10" width="19" style="19" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="14.5" style="19"/>
+    <col min="1" max="9" width="14.5" style="13"/>
+    <col min="10" max="10" width="19" style="13" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="14.5" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="21" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="23" t="s">
+      <c r="Q1" s="35"/>
+      <c r="R1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="22"/>
-      <c r="T1" s="23" t="s">
+      <c r="S1" s="35"/>
+      <c r="T1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="22"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A2" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="25" t="s">
+      <c r="O2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="S2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="25" t="s">
+      <c r="T2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="U2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="V2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="W2" s="26" t="s">
+      <c r="W2" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A3" s="27"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="28">
-        <f>C3-G3</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="27">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="19">
+        <f t="shared" ref="F3:F32" si="0">C3-G3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="18">
         <v>43983</v>
       </c>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="28">
-        <f>C4-G4</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="27">
+      <c r="A4" s="18"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="18">
         <v>43984</v>
       </c>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A5" s="27"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="28">
-        <f>C5-G5</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="27">
+      <c r="A5" s="18"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="18">
         <v>43985</v>
       </c>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="28" t="s">
+      <c r="P5" s="19"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="19" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A6" s="27"/>
-      <c r="B6" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="28">
-        <f>C6-G6</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="27">
+      <c r="A6" s="18"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="18">
         <v>43986</v>
       </c>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="28" t="s">
+      <c r="P6" s="19"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="Y6" s="28">
+      <c r="Y6" s="19">
         <f>SUM(C3:C32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A7" s="27"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="28">
-        <f>C7-G7</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="27">
+      <c r="A7" s="18"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="18">
         <v>43987</v>
       </c>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="28"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="28" t="s">
+      <c r="P7" s="19"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="Y7" s="28">
+      <c r="Y7" s="19">
         <f>SUM(I3:I31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A8" s="27"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="28">
-        <f>C8-G8</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="27">
+      <c r="A8" s="18"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="18">
         <v>43988</v>
       </c>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28"/>
-      <c r="U8" s="28"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="28" t="s">
+      <c r="P8" s="19"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="Y8" s="30">
+      <c r="Y8" s="21">
         <v>242609.17</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A9" s="27"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="28">
-        <f>C9-G9</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="27">
+      <c r="A9" s="18"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="18">
         <v>43989</v>
       </c>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="28" t="s">
+      <c r="P9" s="19"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="Y9" s="30">
+      <c r="Y9" s="21">
         <v>1180834.3600000001</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A10" s="27"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="28">
-        <f>C10-G10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="27">
+      <c r="A10" s="18"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="18">
         <v>43990</v>
       </c>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="28"/>
-      <c r="T10" s="28"/>
-      <c r="U10" s="28"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="19" t="s">
+      <c r="P10" s="19"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="Y10" s="30">
+      <c r="Y10" s="21">
         <v>77682.600000000006</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A11" s="27"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="28">
-        <f>C11-G11</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="27">
+      <c r="A11" s="18"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="18">
         <v>43991</v>
       </c>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="28"/>
-      <c r="U11" s="28"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A12" s="27"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="28">
-        <f>C12-G12</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="27">
+      <c r="A12" s="18"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="18">
         <v>43992</v>
       </c>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="Y12" s="30">
+      <c r="P12" s="19"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="Y12" s="21">
         <f>Y6-Y7-Y8-F4</f>
         <v>-242609.17</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A13" s="27"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="28">
-        <f>C13-G13</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="27">
+      <c r="A13" s="18"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="18">
         <v>43993</v>
       </c>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="28"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A14" s="27"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="28">
-        <f>C14-G14</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="27">
+      <c r="A14" s="18"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="18">
         <v>43994</v>
       </c>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="28"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="Y14" s="30">
+      <c r="P14" s="19"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="Y14" s="21">
         <f>Q36</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A15" s="27"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="28">
-        <f>C15-G15</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="27">
+      <c r="A15" s="18"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="18">
         <v>43995</v>
       </c>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="28"/>
-      <c r="S15" s="28"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A16" s="27"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="28">
-        <f>C16-G16</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="27">
+      <c r="A16" s="18"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="18">
         <v>43996</v>
       </c>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="28"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="28"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="Y16" s="31">
+      <c r="P16" s="19"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="Y16" s="22">
         <f>Y7</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A17" s="27"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="28">
-        <f>C17-G17</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="27">
+      <c r="A17" s="18"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="18">
         <v>43997</v>
       </c>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A18" s="27"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="28">
-        <f>C18-G18</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="27">
+      <c r="A18" s="18"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="18">
         <v>43998</v>
       </c>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="28"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="28">
-        <f>C19-G19</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="27">
+      <c r="A19" s="18"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="18">
         <v>43999</v>
       </c>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="28"/>
-      <c r="S19" s="28"/>
-      <c r="T19" s="28"/>
-      <c r="U19" s="28"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
     </row>
     <row r="20" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A20" s="27"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="28">
-        <f>C20-G20</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="27">
+      <c r="A20" s="18"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="18">
         <v>44000</v>
       </c>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="28"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
     </row>
     <row r="21" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A21" s="27"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="28">
-        <f>C21-G21</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="27">
+      <c r="A21" s="18"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="18">
         <v>44001</v>
       </c>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="28"/>
-      <c r="T21" s="28"/>
-      <c r="U21" s="28"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
     </row>
     <row r="22" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A22" s="27"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="28">
-        <f>C22-G22</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="27">
+      <c r="A22" s="18"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="18">
         <v>44002</v>
       </c>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="28"/>
-      <c r="S22" s="28"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="28"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
     </row>
     <row r="23" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A23" s="27"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="28">
-        <f>C23-G23</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="27">
+      <c r="A23" s="18"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="18">
         <v>44003</v>
       </c>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="28"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="28"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
     </row>
     <row r="24" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A24" s="27"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="28">
-        <f>C24-G24</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="27">
+      <c r="A24" s="18"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="18">
         <v>44004</v>
       </c>
-      <c r="P24" s="28"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="28"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
     </row>
     <row r="25" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A25" s="27"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="28">
-        <f>C25-G25</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="27">
+      <c r="A25" s="18"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="18">
         <v>44005</v>
       </c>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="28"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="24"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
     </row>
     <row r="26" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A26" s="27"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="28">
-        <f>C26-G26</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="27">
+      <c r="A26" s="18"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="18">
         <v>44006</v>
       </c>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="28"/>
-      <c r="S26" s="28"/>
-      <c r="T26" s="28"/>
-      <c r="U26" s="28"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
     </row>
     <row r="27" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A27" s="27"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="28">
-        <f>C27-G27</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="27">
+      <c r="A27" s="18"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="18">
         <v>44007</v>
       </c>
-      <c r="P27" s="28"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="28"/>
-      <c r="S27" s="28"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="28"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
     </row>
     <row r="28" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A28" s="27"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="28">
-        <f>C28-G28</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="27">
+      <c r="A28" s="18"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="18">
         <v>44008</v>
       </c>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="28"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="28"/>
-      <c r="U28" s="28"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="24"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
     </row>
     <row r="29" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A29" s="27"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="28">
-        <f>C29-G29</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="27">
+      <c r="A29" s="18"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="18">
         <v>44009</v>
       </c>
-      <c r="P29" s="28"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="28"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="28"/>
-      <c r="U29" s="28"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="24"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
     </row>
     <row r="30" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A30" s="27"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="28">
-        <f>C30-G30</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="27">
+      <c r="A30" s="18"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="18">
         <v>44010</v>
       </c>
-      <c r="P30" s="28"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="28"/>
-      <c r="S30" s="28"/>
-      <c r="T30" s="28"/>
-      <c r="U30" s="28"/>
-      <c r="V30" s="24"/>
-      <c r="W30" s="24"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
     </row>
     <row r="31" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A31" s="27"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="28">
-        <f>C31-G31</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="27">
+      <c r="A31" s="18"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="18">
         <v>44011</v>
       </c>
-      <c r="P31" s="28"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="28"/>
-      <c r="S31" s="28"/>
-      <c r="T31" s="28"/>
-      <c r="U31" s="28"/>
-      <c r="V31" s="24"/>
-      <c r="W31" s="24"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="15"/>
     </row>
     <row r="32" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A32" s="27"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="28">
-        <f>C32-G32</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="L32" s="33"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="27">
+      <c r="A32" s="18"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="L32" s="24"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="18">
         <v>44012</v>
       </c>
-      <c r="P32" s="28"/>
-      <c r="Q32" s="28"/>
-      <c r="R32" s="28"/>
-      <c r="S32" s="28"/>
-      <c r="T32" s="28"/>
-      <c r="U32" s="28"/>
-      <c r="V32" s="24"/>
-      <c r="W32" s="24"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="15"/>
     </row>
     <row r="33" spans="2:23" ht="15.75" customHeight="1">
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="33"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="34" t="s">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="24"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="P33" s="35">
-        <f t="shared" ref="P33:W33" si="0">SUM(P3:P32)</f>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R33" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S33" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T33" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U33" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V33" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W33" s="35">
-        <f t="shared" si="0"/>
+      <c r="P33" s="26">
+        <f t="shared" ref="P33:W33" si="1">SUM(P3:P32)</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R33" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S33" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T33" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U33" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V33" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W33" s="26">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:23" ht="15.75" customHeight="1">
-      <c r="L34" s="33"/>
-      <c r="M34" s="24"/>
-      <c r="N34" s="26"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="17"/>
     </row>
     <row r="35" spans="2:23" ht="15.75" customHeight="1">
-      <c r="L35" s="33"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="26"/>
-      <c r="P35" s="28"/>
-      <c r="W35" s="28">
+      <c r="L35" s="24"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="17"/>
+      <c r="P35" s="19"/>
+      <c r="W35" s="19">
         <f>SUM(W3:W32)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:23" ht="15.75" customHeight="1">
-      <c r="L36" s="33"/>
-      <c r="M36" s="24"/>
-      <c r="N36" s="24"/>
-      <c r="Q36" s="28"/>
-      <c r="W36" s="30">
+      <c r="L36" s="24"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="Q36" s="19"/>
+      <c r="W36" s="21">
         <v>320291.77</v>
       </c>
     </row>
     <row r="37" spans="2:23" ht="15.75" customHeight="1">
-      <c r="L37" s="24"/>
-      <c r="M37" s="24"/>
-      <c r="N37" s="24"/>
-      <c r="W37" s="30">
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="W37" s="21">
         <f>W35-W36</f>
         <v>-320291.77</v>
       </c>

</xml_diff>